<commit_message>
Additional test for submission_test_file_from_doug_20231130.xlsx.
</commit_message>
<xml_diff>
--- a/src/encoded/tests/data/test-files/submission_test_file_from_doug_20231130.xlsx
+++ b/src/encoded/tests/data/test-files/submission_test_file_from_doug_20231130.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmichaels/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmichaels/repos/cgap/smaht-portal/src/encoded/tests/data/test-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF4CF250-CA0B-7445-A8BF-9E55B36A8F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9592961D-6547-264D-8B53-AD52CD6DAFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{E8407000-4AC9-C547-896C-C1D84CEDAAF5}"/>
   </bookViews>
   <sheets>
-    <sheet name="donor" sheetId="2" r:id="rId1"/>
+    <sheet name="donor " sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>

</xml_diff>